<commit_message>
ran completeness test for NuSEDS
</commit_message>
<xml_diff>
--- a/DQS_Log_Beta.xlsx
+++ b/DQS_Log_Beta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1980,6 +1980,447 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:16:51</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>POPULATION, ESTIMATE_CLASSIFICATION, ESTIMATE_METHOD</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Consistency (C1)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:17:07</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.9946666666666667</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>POPULATION, ESTIMATE_CLASSIFICATION, ESTIMATE_METHOD</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Consistency (C1)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:17:18</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.9946666666666667</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>AREA, ANALYSIS_YR, NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER, EFFECTIVE_FEMALES, WEIGHTED_PCT_SPAWN, NO_INSPECTIONS_USED, ACT_ID, POP_ID, GFE_ID</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:17:19</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Accuracy (A2)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:17:29</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:17:40</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>North and Central Coast NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:18:57</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>West Coast Vancouver Island NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:19:26</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:20:13</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Completeness (C1)</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:25:08</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.9153491436100132</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>West Coast Vancouver Island NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Completeness (C1)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:26:35</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.888227784909428</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>North and Central Coast NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Completeness (C1)</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:27:50</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.8610714086106374</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Completeness (C1)</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2024-11-29 16:28:36</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.8482207305966877</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ran 5 tests for habitat restoration and head depots
</commit_message>
<xml_diff>
--- a/DQS_Log_Beta.xlsx
+++ b/DQS_Log_Beta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2421,6 +2421,788 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>POPULATION, ESTIMATE_CLASSIFICATION, ESTIMATE_METHOD</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Consistency (C1)</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2024-12-02 13:55:13</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.9946666666666667</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>AREA, ANALYSIS_YR, NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER, EFFECTIVE_FEMALES, WEIGHTED_PCT_SPAWN, NO_INSPECTIONS_USED, ACT_ID, POP_ID, GFE_ID</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2024-12-02 13:55:14</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Accuracy (A2)</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2024-12-02 13:55:28</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2024-12-02 13:55:28</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2024-12-02 13:55:41</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.8482207305966877</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>site_species_id, project_name, project_description, ecosystem_type, species_name, CU_Name, SMU_Display, SMU_ID</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Consistency (C1)</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2024-12-02 14:56:59</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.9206204379562044</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>AREA, ANALYSIS_YR, NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER, EFFECTIVE_FEMALES, WEIGHTED_PCT_SPAWN, NO_INSPECTIONS_USED, ACT_ID, POP_ID, GFE_ID</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2024-12-02 14:57:00</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Accuracy (A2)</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2024-12-02 14:57:11</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Yukon and Transboundary NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2024-12-02 14:57:12</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Johnstone Strait and Strait of Georgia NuSEDS_20241004</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2024-12-02 14:57:24</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.8482207305966877</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2024-12-02 14:59:48</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:00:24</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>site_latitude, site_longitude</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Accuracy (A2)</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:00:25</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:00:25</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:00:25</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.7664092664092664</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:01:13</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:01:47</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:02:09</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>SalmonHabitatRestorationProjects_DataPortal_June_FinalFields_20240613</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:02:33</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Pacific-Recreational-Fishery-Salmon-Head-Depots</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DEPOT NAME / NOM DU DÉPÔT, AREA / LA RÉGION, MUNICIPALITY / MUNICIPALITÉ, ADDRESS / ADRESSE, STORAGE INFORMATION / DÉTAILS DE STOCKAGE</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Consistency (C1)</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:31:28</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Pacific-Recreational-Fishery-Salmon-Head-Depots</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>LATITUDE / LATITUDE, LONGITUDE / LONGITUDE</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:31:28</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Pacific-Recreational-Fishery-Salmon-Head-Depots</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>LATITUDE / LATITUDE, LONGITUDE / LONGITUDE</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Accuracy (A2)</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:31:28</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F86" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Pacific-Recreational-Fishery-Salmon-Head-Depots</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:31:28</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Pacific-Recreational-Fishery-Salmon-Head-Depots</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2024-12-02 15:31:28</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.9764764764764765</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>EwertM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Global variables and fixed A2
</commit_message>
<xml_diff>
--- a/DQS_Log_Beta.xlsx
+++ b/DQS_Log_Beta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2421,6 +2421,212 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>CU_Name</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Consistency (C1)</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2024-12-02 23:10:16</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Shape_Length, Shape_Area</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2024-12-02 23:10:16</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>0.993670886075949</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ACT_ID, ANALYSIS_YR, STREAM_ID, SPL_ID, NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER, UNSPECIFIED_RETURN, NO_INSPECTIONS_USED, MAX_ESTIMATE, EFFECTIVE_FEMALES, WEIGHTED_PCT_SPAWN, OTHER_ADULT_REMOVALS, OTHER_JACK_REMOVALS, TOT_ADULT_RET_RIVER, POP_ID, SBJ_ID</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2024-12-03 09:00:49</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>onakd</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2024-12-03 09:02:20</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>onakd</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2024-12-03 09:02:40</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.924034635876363</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>onakd</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ACT_ID, ANALYSIS_YR, STREAM_ID, SPL_ID, NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER, UNSPECIFIED_RETURN, NO_INSPECTIONS_USED, MAX_ESTIMATE, EFFECTIVE_FEMALES, WEIGHTED_PCT_SPAWN, OTHER_ADULT_REMOVALS, OTHER_JACK_REMOVALS, TOT_ADULT_RET_RIVER, TOT_JACK_RET_RIVER, JUV_PRES_TYP, POP_ID, SBJ_ID</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2024-12-03 09:07:44</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>0.9965248818459828</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>onakd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added utils folder and error handeling
</commit_message>
<xml_diff>
--- a/DQS_Log_Beta.xlsx
+++ b/DQS_Log_Beta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2627,6 +2627,336 @@
         </is>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:55</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:56</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:06:56</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:31</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:31</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>CK_CU_BOUNDARY_En</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:13:31</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>ACT_ID, ANALYSIS_YR, STREAM_ID, SPL_ID, NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER, UNSPECIFIED_RETURN, NO_INSPECTIONS_USED, MAX_ESTIMATE, EFFECTIVE_FEMALES, WEIGHTED_PCT_SPAWN, OTHER_ADULT_REMOVALS, OTHER_JACK_REMOVALS, TOT_ADULT_RET_RIVER, TOT_JACK_RET_RIVER, JUV_PRES_TYP, POP_ID, SBJ_ID</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Accuracy (A1)</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:15:28</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>0.9968144750254843</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>ACT_ID, ANALYSIS_YR, STREAM_ID, SPL_ID, NATURAL_ADULT_SPAWNERS, NATURAL_JACK_SPAWNERS, NATURAL_SPAWNERS_TOTAL, ADULT_BROODSTOCK_REMOVALS, JACK_BROODSTOCK_REMOVALS, TOTAL_BROODSTOCK_REMOVALS, OTHER_REMOVALS, TOTAL_RETURN_TO_RIVER, UNSPECIFIED_RETURN, NO_INSPECTIONS_USED, MAX_ESTIMATE, EFFECTIVE_FEMALES, WEIGHTED_PCT_SPAWN, OTHER_ADULT_REMOVALS, OTHER_JACK_REMOVALS, TOT_ADULT_RET_RIVER, TOT_JACK_RET_RIVER, JUV_PRES_TYP, POP_ID, SBJ_ID</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Accuracy (A2)</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:15:29</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Accuracy (A3)</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:15:31</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>no threshold</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Conservation_Unit_Data_20220902</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>All columns</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Completeness (P)</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2024-12-03 12:15:32</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.9240346358763629</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>OnakD</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>